<commit_message>
Update online jewellery shopping app.xlsx
</commit_message>
<xml_diff>
--- a/Extra Work/online jewellery shopping app.xlsx
+++ b/Extra Work/online jewellery shopping app.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenario" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="156">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -595,6 +595,96 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1AazCS6oM4p_JtkChmBwtZY7XEDDCpZtr/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>check faq button</t>
+  </si>
+  <si>
+    <t>1) open the google play store
+2) search the online shopping jewellery app name
+3) install the jewellery onlin shopping app
+4) open the jewellery online shopping app
+5) click on left side menu icon
+6) click on  help center menu
+7) click on faq button</t>
+  </si>
+  <si>
+    <t>while clicking on faq button it is working properly an d also have opened.</t>
+  </si>
+  <si>
+    <t>check order queries button</t>
+  </si>
+  <si>
+    <t>1) open the google play store
+2) search the online shopping jewellery app name
+3) install the jewellery onlin shopping app
+4) open the jewellery online shopping app
+5) click on left side menu icon
+6) click on  help center menu
+7) click on order queries button</t>
+  </si>
+  <si>
+    <t>while clicking on order queries button it is working properly and also have opened.</t>
+  </si>
+  <si>
+    <t>check payment/returns button</t>
+  </si>
+  <si>
+    <t>1) open the google play store
+2) search the online shopping jewellery app name
+3) install the jewellery onlin shopping app
+4) open the jewellery online shopping app
+5) click on left side menu icon
+6) click on  help center menu
+7) click on payment/returns button</t>
+  </si>
+  <si>
+    <t>while clicking on payment/returns button it is working properly and also have opened.</t>
+  </si>
+  <si>
+    <t>check wallet/coupon button</t>
+  </si>
+  <si>
+    <t>1) open the google play store
+2) search the online shopping jewellery app name
+3) install the jewellery onlin shopping app
+4) open the jewellery online shopping app
+5) click on left side menu icon
+6) click on  help center menu
+7) click on wallet/coupon button</t>
+  </si>
+  <si>
+    <t>while clicking on wallet/coupon button it is working properly and also have opened.</t>
+  </si>
+  <si>
+    <t>check others button</t>
+  </si>
+  <si>
+    <t>1) open the google play store
+2) search the online shopping jewellery app name
+3) install the jewellery onlin shopping app
+4) open the jewellery online shopping app
+5) click on left side menu icon
+6) click on  help center menu
+7) click on others button</t>
+  </si>
+  <si>
+    <t>while clicking on others button it is working properly and also have opened.</t>
+  </si>
+  <si>
+    <t>check read our faqs button</t>
+  </si>
+  <si>
+    <t>1) open the google play store
+2) search the online shopping jewellery app name
+3) install the jewellery onlin shopping app
+4) open the jewellery online shopping app
+5) click on left side menu icon
+6) click on  help center menu
+7) click on read our faqs button</t>
+  </si>
+  <si>
+    <t>while clicking on read faqs button it is working properly and also have opened.</t>
   </si>
 </sst>
 </file>
@@ -683,7 +773,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -736,21 +826,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1101,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,6 +2217,180 @@
         <v>14</v>
       </c>
     </row>
+    <row r="36" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7">
+        <v>35</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="H36" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7">
+        <v>36</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7">
+        <v>37</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7">
+        <v>38</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7">
+        <v>39</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7">
+        <v>40</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="H41" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2143,8 +2401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>